<commit_message>
few more in arrays
</commit_message>
<xml_diff>
--- a/interivew/practice/tracker.xlsx
+++ b/interivew/practice/tracker.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="457">
   <si>
     <t>LIS</t>
   </si>
@@ -1336,6 +1336,69 @@
   </si>
   <si>
     <t>Stock-maxProfitWithKTransactions</t>
+  </si>
+  <si>
+    <t>CheckIfArrayIsArthimaticSequence</t>
+  </si>
+  <si>
+    <t>CountAllPairsWithGivenDifferenceX</t>
+  </si>
+  <si>
+    <t>FindIncreasingSequenceOfLength3WithMaxProduct</t>
+  </si>
+  <si>
+    <t>FindMinInSortedRotatedArray</t>
+  </si>
+  <si>
+    <t>FindSubarrayOfSumZero</t>
+  </si>
+  <si>
+    <t>MoveAllZeroesToEndOfArray</t>
+  </si>
+  <si>
+    <t>CheckForOverflow</t>
+  </si>
+  <si>
+    <t>FindCommonMinInTwoArrays</t>
+  </si>
+  <si>
+    <t>HashMapCustom</t>
+  </si>
+  <si>
+    <t>InfixToPostfix</t>
+  </si>
+  <si>
+    <t>PostfixEval</t>
+  </si>
+  <si>
+    <t>FindKthNodeInBinaryTree</t>
+  </si>
+  <si>
+    <t>CheckForDuplicatesWithInKDistance</t>
+  </si>
+  <si>
+    <t>FindFirstRepeatingNumber</t>
+  </si>
+  <si>
+    <t>MaxSumPathSumInTwoArrays</t>
+  </si>
+  <si>
+    <t>PrintDistinctElementsInArray</t>
+  </si>
+  <si>
+    <t>RemoveElementFromArray</t>
+  </si>
+  <si>
+    <t>ReplaceWithLeftRightMultiplication</t>
+  </si>
+  <si>
+    <t>XPowerN</t>
+  </si>
+  <si>
+    <t>SortArrayByAnotherArray</t>
+  </si>
+  <si>
+    <t>AVLTreeNodeWithCount</t>
   </si>
 </sst>
 </file>
@@ -2044,8 +2107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2967,61 +3030,97 @@
       <c r="A71" s="6" t="s">
         <v>96</v>
       </c>
+      <c r="C71" t="s">
+        <v>436</v>
+      </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
         <v>97</v>
       </c>
+      <c r="C72" t="s">
+        <v>437</v>
+      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="6" t="s">
         <v>98</v>
       </c>
+      <c r="C73" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="6" t="s">
         <v>99</v>
       </c>
+      <c r="C74" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="7" t="s">
         <v>100</v>
       </c>
+      <c r="C75" t="s">
+        <v>440</v>
+      </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
         <v>101</v>
       </c>
+      <c r="C76" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="s">
         <v>102</v>
       </c>
+      <c r="C77" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
         <v>103</v>
       </c>
+      <c r="C78" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="9" t="s">
         <v>104</v>
       </c>
+      <c r="C79" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
         <v>105</v>
       </c>
+      <c r="C80" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="15" t="s">
         <v>106</v>
       </c>
+      <c r="C81" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="6" t="s">
         <v>107</v>
       </c>
+      <c r="C82" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
@@ -3182,7 +3281,7 @@
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A114" s="4" t="s">
+      <c r="A114" s="8" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3304,10 +3403,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H106"/>
+  <dimension ref="B1:H111"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3355,8 +3454,8 @@
       <c r="B5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>271</v>
+      <c r="D5" t="s">
+        <v>450</v>
       </c>
       <c r="H5" s="4"/>
     </row>
@@ -3364,36 +3463,54 @@
       <c r="B6" s="6" t="s">
         <v>48</v>
       </c>
+      <c r="D6" t="s">
+        <v>451</v>
+      </c>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>202</v>
       </c>
+      <c r="D7" t="s">
+        <v>452</v>
+      </c>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>203</v>
       </c>
+      <c r="D8" t="s">
+        <v>453</v>
+      </c>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>205</v>
       </c>
+      <c r="D9" t="s">
+        <v>454</v>
+      </c>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>206</v>
       </c>
+      <c r="D10" t="s">
+        <v>455</v>
+      </c>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="6" t="s">
         <v>74</v>
       </c>
+      <c r="D11" t="s">
+        <v>456</v>
+      </c>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.35">
@@ -3539,7 +3656,9 @@
       <c r="B41" s="4"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B42" s="4"/>
+      <c r="B42" s="4" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B43" s="4" t="s">
@@ -3601,212 +3720,233 @@
         <v>128</v>
       </c>
     </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B55" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B56" s="4" t="s">
-        <v>59</v>
+      <c r="B56" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B57" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B58" s="4" t="s">
-        <v>35</v>
-      </c>
+      <c r="B57" s="4"/>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B59" s="4" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B60" s="4" t="s">
-        <v>207</v>
+        <v>30</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B61" s="4" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B62" s="4"/>
+      <c r="B62" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B63" s="4" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B64" s="4" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B65" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B66" s="4"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B67" s="4"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B69" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B70" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B66" s="4" t="s">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B71" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B67" s="4" t="s">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B72" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B68" s="4" t="s">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B73" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B73" s="6" t="s">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B78" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B74" s="6" t="s">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B79" s="6" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B75" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B76" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B77" s="4"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B78" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B79" s="4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B80" s="4" t="s">
-        <v>91</v>
+        <v>201</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B81" s="4" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B82" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="B82" s="4"/>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B83" s="4" t="s">
-        <v>75</v>
+        <v>129</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B84" s="4" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B85" s="4" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B86" s="4" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B87" s="4" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B88" s="4" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B89" s="1" t="s">
-        <v>272</v>
+      <c r="B89" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B90" s="9" t="s">
-        <v>121</v>
+      <c r="B90" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B91" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B92" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B93" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B94" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B95" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B96" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B92" s="9"/>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B95" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B96" s="1" t="s">
-        <v>400</v>
-      </c>
-    </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B97" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B98" s="1" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B99" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="B97" s="9"/>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B100" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B101" s="1" t="s">
-        <v>404</v>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B102" s="1" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B103" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B104" s="1" t="s">
-        <v>362</v>
+        <v>16</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B105" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B106" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B108" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B109" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B110" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B111" s="1" t="s">
         <v>407</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reg exp in java
</commit_message>
<xml_diff>
--- a/interivew/practice/tracker.xlsx
+++ b/interivew/practice/tracker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9400" windowHeight="7900" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9400" windowHeight="7900" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="topics" sheetId="12" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="464">
   <si>
     <t>LIS</t>
   </si>
@@ -1417,13 +1417,16 @@
   </si>
   <si>
     <t>Yet</t>
+  </si>
+  <si>
+    <t>Pascal Triangle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1517,6 +1520,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1577,7 +1588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1604,6 +1615,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2151,8 +2163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4125,8 +4137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4164,7 +4176,7 @@
       <c r="C3" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="24" t="s">
         <v>216</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -4198,7 +4210,7 @@
       <c r="C5" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="24" t="s">
         <v>220</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -4305,6 +4317,9 @@
       <c r="A12" s="1" t="s">
         <v>222</v>
       </c>
+      <c r="D12" s="1" t="s">
+        <v>463</v>
+      </c>
       <c r="F12" s="1" t="s">
         <v>243</v>
       </c>
@@ -4331,6 +4346,7 @@
       <c r="A16" s="3" t="s">
         <v>226</v>
       </c>
+      <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">

</xml_diff>

<commit_message>
Graphs - Detect Cycle
</commit_message>
<xml_diff>
--- a/interivew/practice/tracker.xlsx
+++ b/interivew/practice/tracker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9400" windowHeight="7900" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9400" windowHeight="7900" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="topics" sheetId="12" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="478">
   <si>
     <t>LIS</t>
   </si>
@@ -1423,6 +1423,45 @@
   </si>
   <si>
     <t>Fibonacci Applications</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>GraphTraversals - DFS</t>
+  </si>
+  <si>
+    <t>GraphTraversals - BFS</t>
+  </si>
+  <si>
+    <t>Detect Cycle in Undirected Graph - UnionFind</t>
+  </si>
+  <si>
+    <t>Detect Cycle in Undirected Graph - DFS</t>
+  </si>
+  <si>
+    <t>Detect Cycle in Directed Graph</t>
+  </si>
+  <si>
+    <t>Matrix</t>
+  </si>
+  <si>
+    <t>CheckForDuplicatesWithInKDistanceOfMatrix</t>
+  </si>
+  <si>
+    <t>Search in a row wise and column wise sorted matrix</t>
+  </si>
+  <si>
+    <t>Print a given matrix in spiral form</t>
+  </si>
+  <si>
+    <t>Print unique rows in a given boolean matrix</t>
+  </si>
+  <si>
+    <t>Rotate Matrix Elements</t>
+  </si>
+  <si>
+    <t>A Boolean Matrix Question (MakeRowsAndColumns1IfCellIs1)</t>
   </si>
 </sst>
 </file>
@@ -2164,10 +2203,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G136"/>
+  <dimension ref="A2:K136"/>
   <sheetViews>
-    <sheetView topLeftCell="C53" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2176,10 +2215,13 @@
     <col min="2" max="2" width="8.7265625" style="1"/>
     <col min="3" max="5" width="42.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="79.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1"/>
+    <col min="7" max="9" width="8.7265625" style="1"/>
+    <col min="10" max="10" width="38.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="53.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>165</v>
       </c>
@@ -2195,8 +2237,14 @@
       <c r="F2" s="5" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J2" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
@@ -2212,8 +2260,14 @@
       <c r="F3" s="12" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J3" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>32</v>
       </c>
@@ -2229,8 +2283,14 @@
       <c r="F4" s="12" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J4" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>33</v>
       </c>
@@ -2246,8 +2306,14 @@
       <c r="F5" s="12" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J5" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>34</v>
       </c>
@@ -2266,8 +2332,14 @@
       <c r="G6" s="1" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J6" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>35</v>
       </c>
@@ -2286,8 +2358,14 @@
       <c r="G7" s="1" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J7" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>36</v>
       </c>
@@ -2306,8 +2384,11 @@
       <c r="G8" s="1" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K8" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>29</v>
       </c>
@@ -2323,8 +2404,11 @@
       <c r="F9" s="12" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K9" s="1" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>37</v>
       </c>
@@ -2340,8 +2424,11 @@
       <c r="F10" s="16" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K10" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>38</v>
       </c>
@@ -2358,7 +2445,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>39</v>
       </c>
@@ -2375,7 +2462,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>40</v>
       </c>
@@ -2392,7 +2479,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>41</v>
       </c>
@@ -2409,7 +2496,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="20" t="s">
         <v>42</v>
       </c>
@@ -2426,7 +2513,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>43</v>
       </c>
@@ -3521,8 +3608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3860,14 +3947,10 @@
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B60" s="4" t="s">
-        <v>394</v>
-      </c>
+      <c r="B60" s="4"/>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B61" s="4" t="s">
-        <v>395</v>
-      </c>
+      <c r="B61" s="4"/>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B62" s="4"/>
@@ -4149,7 +4232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="C2:F13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
backtracking and practice in bsts
</commit_message>
<xml_diff>
--- a/interivew/practice/tracker.xlsx
+++ b/interivew/practice/tracker.xlsx
@@ -9,14 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9400" windowHeight="7900" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9400" windowHeight="7900" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="topics" sheetId="12" r:id="rId1"/>
-    <sheet name="All" sheetId="5" r:id="rId2"/>
-    <sheet name="practice" sheetId="11" r:id="rId3"/>
-    <sheet name="groups" sheetId="13" r:id="rId4"/>
-    <sheet name="dp" sheetId="14" r:id="rId5"/>
+    <sheet name="practice" sheetId="11" r:id="rId2"/>
+    <sheet name="groups" sheetId="13" r:id="rId3"/>
+    <sheet name="dp" sheetId="14" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,86 +27,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="458">
   <si>
     <t>LIS</t>
   </si>
   <si>
-    <t>Wordwrap</t>
-  </si>
-  <si>
-    <t>Basic</t>
-  </si>
-  <si>
     <t>LCS</t>
   </si>
   <si>
-    <t>Knapsack</t>
-  </si>
-  <si>
-    <t>Subset Sum</t>
-  </si>
-  <si>
-    <t>MaxContiguous Sum</t>
-  </si>
-  <si>
-    <t>MaxIncreasing Sequence</t>
-  </si>
-  <si>
-    <t>MinCost</t>
-  </si>
-  <si>
-    <t>Intermediate</t>
-  </si>
-  <si>
-    <t>Edit</t>
-  </si>
-  <si>
-    <t>Boxstack</t>
-  </si>
-  <si>
-    <t>Rodcut</t>
-  </si>
-  <si>
-    <t>Longest Palindrome</t>
-  </si>
-  <si>
-    <t>LongestBitonic</t>
-  </si>
-  <si>
     <t>Matrix Chain Multiplication</t>
   </si>
   <si>
     <t>PalindromePartition</t>
   </si>
   <si>
-    <t>Partition Problem</t>
-  </si>
-  <si>
-    <t>Advanced</t>
-  </si>
-  <si>
-    <t>MaxlengthofChainOfPairs</t>
-  </si>
-  <si>
-    <t>Egg Dropping</t>
-  </si>
-  <si>
-    <t>Floyd Marshall</t>
-  </si>
-  <si>
-    <t>Fib other ways</t>
-  </si>
-  <si>
-    <t>Ugly</t>
-  </si>
-  <si>
-    <t>Bellman-Ford</t>
-  </si>
-  <si>
-    <t>Largest Independent Set</t>
-  </si>
-  <si>
     <t>Boolean Parenthesization Problem</t>
   </si>
   <si>
@@ -543,15 +476,6 @@
     <t>Bit algorithms</t>
   </si>
   <si>
-    <t>binary(Count-23)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      bst(Count-22)</t>
-  </si>
-  <si>
-    <t>linkedlist(Count-21)</t>
-  </si>
-  <si>
     <t>Binary Search</t>
   </si>
   <si>
@@ -1462,13 +1386,28 @@
   </si>
   <si>
     <t>A Boolean Matrix Question (MakeRowsAndColumns1IfCellIs1)</t>
+  </si>
+  <si>
+    <t>binary(Count-23) - 41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      bst(Count-22) - 38</t>
+  </si>
+  <si>
+    <t>linkedlist(Count-21) - 41</t>
+  </si>
+  <si>
+    <t>Matrix Multiplication</t>
+  </si>
+  <si>
+    <t>Mathetmatical</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1570,6 +1509,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1630,7 +1577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1658,6 +1605,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1969,7 +1917,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection sqref="A1:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1980,83 +1928,83 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>274</v>
+        <v>249</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>312</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>275</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>276</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2066,147 +2014,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="23.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2223,1102 +2034,1102 @@
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>198</v>
-      </c>
       <c r="J2" s="5" t="s">
-        <v>465</v>
+        <v>440</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>471</v>
+        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>314</v>
+        <v>289</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>323</v>
+        <v>298</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>466</v>
+        <v>441</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>473</v>
+        <v>448</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>315</v>
+        <v>290</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>324</v>
+        <v>299</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>467</v>
+        <v>442</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>474</v>
+        <v>449</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>304</v>
+        <v>279</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>316</v>
+        <v>291</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>349</v>
+        <v>324</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>468</v>
+        <v>443</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>477</v>
+        <v>452</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>279</v>
+        <v>254</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>317</v>
+        <v>292</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>348</v>
+        <v>323</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>386</v>
+        <v>361</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>469</v>
+        <v>444</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>313</v>
+        <v>288</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>350</v>
+        <v>325</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>387</v>
+        <v>362</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>470</v>
+        <v>445</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>318</v>
+        <v>293</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>351</v>
+        <v>326</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>388</v>
+        <v>363</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>282</v>
+        <v>257</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>319</v>
+        <v>294</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>353</v>
+        <v>328</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>476</v>
+        <v>451</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>283</v>
+        <v>258</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>320</v>
+        <v>295</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>352</v>
+        <v>327</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>472</v>
+        <v>447</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>284</v>
+        <v>259</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>321</v>
+        <v>296</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>354</v>
+        <v>329</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>285</v>
+        <v>260</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>322</v>
+        <v>297</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>355</v>
+        <v>330</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>323</v>
+        <v>298</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>357</v>
+        <v>332</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>287</v>
+        <v>262</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>324</v>
+        <v>299</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>356</v>
+        <v>331</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="20" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>288</v>
+        <v>263</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>325</v>
+        <v>300</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>360</v>
+        <v>335</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>289</v>
+        <v>264</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>326</v>
+        <v>301</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>359</v>
+        <v>334</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>290</v>
+        <v>265</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>327</v>
+        <v>302</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>358</v>
+        <v>333</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>291</v>
+        <v>266</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>328</v>
+        <v>303</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>362</v>
+        <v>337</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="20" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>292</v>
+        <v>267</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>419</v>
+        <v>394</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>361</v>
+        <v>336</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>301</v>
+        <v>276</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>329</v>
+        <v>304</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>363</v>
+        <v>338</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>330</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>365</v>
+        <v>340</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>293</v>
+        <v>268</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>331</v>
+        <v>306</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>364</v>
+        <v>339</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>294</v>
+        <v>269</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>334</v>
+        <v>309</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>366</v>
+        <v>341</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="19" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>296</v>
+        <v>271</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>333</v>
+        <v>308</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>367</v>
+        <v>342</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>295</v>
+        <v>270</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>332</v>
+        <v>307</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>368</v>
+        <v>343</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>306</v>
+        <v>281</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>335</v>
+        <v>310</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>307</v>
+        <v>282</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>336</v>
+        <v>311</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>371</v>
+        <v>346</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>309</v>
+        <v>284</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>337</v>
+        <v>312</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>370</v>
+        <v>345</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>421</v>
+        <v>396</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>373</v>
+        <v>348</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>338</v>
+        <v>313</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>372</v>
+        <v>347</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="20" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>339</v>
+        <v>314</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>410</v>
+        <v>385</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>300</v>
+        <v>275</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>340</v>
+        <v>315</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>415</v>
+        <v>390</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="20" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>310</v>
+        <v>285</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>420</v>
+        <v>395</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>416</v>
+        <v>391</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>311</v>
+        <v>286</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>341</v>
+        <v>316</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>417</v>
+        <v>392</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>302</v>
+        <v>277</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>342</v>
+        <v>317</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>408</v>
+        <v>383</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>303</v>
+        <v>278</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>343</v>
+        <v>318</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>409</v>
+        <v>384</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>353</v>
+        <v>283</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>328</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>411</v>
+        <v>386</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>381</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>345</v>
+        <v>356</v>
+      </c>
+      <c r="D38" s="24" t="s">
+        <v>320</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>412</v>
+        <v>387</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>194</v>
+        <v>169</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>384</v>
+        <v>359</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>344</v>
+        <v>319</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>413</v>
+        <v>388</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>195</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="14" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>426</v>
+        <v>401</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>422</v>
+        <v>397</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>414</v>
+        <v>389</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>196</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>428</v>
+        <v>403</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>346</v>
+        <v>321</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>427</v>
+        <v>402</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>347</v>
+        <v>322</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>429</v>
+        <v>404</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>418</v>
+        <v>393</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>271</v>
+        <v>246</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>449</v>
+        <v>424</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>433</v>
+        <v>408</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>436</v>
+        <v>411</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>434</v>
+        <v>409</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>437</v>
+        <v>412</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="14" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>435</v>
+        <v>410</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>438</v>
+        <v>413</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>374</v>
+        <v>349</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>439</v>
+        <v>414</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="8" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>376</v>
+        <v>351</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>440</v>
+        <v>415</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>375</v>
+        <v>350</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>441</v>
+        <v>416</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>377</v>
+        <v>352</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>442</v>
+        <v>417</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="20" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>432</v>
+        <v>407</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>443</v>
+        <v>418</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>379</v>
+        <v>354</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>444</v>
+        <v>419</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="6" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>382</v>
+        <v>357</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>445</v>
+        <v>420</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="8" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>381</v>
+        <v>356</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>446</v>
+        <v>421</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="6" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>383</v>
+        <v>358</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>447</v>
+        <v>422</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>391</v>
+        <v>366</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>423</v>
+        <v>398</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>464</v>
+        <v>439</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="10" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>424</v>
+        <v>399</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>242</v>
+        <v>217</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="20" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>425</v>
+        <v>400</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>243</v>
+        <v>218</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>430</v>
+        <v>405</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>426</v>
+        <v>401</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="6" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>428</v>
+        <v>403</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>427</v>
+        <v>402</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>429</v>
+        <v>404</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="6" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>431</v>
+        <v>406</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>384</v>
+        <v>359</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="6" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>385</v>
+        <v>360</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="6" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>378</v>
+        <v>353</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="7" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>380</v>
+        <v>355</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="20" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="9" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="14" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="6" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="20" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="8" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="C86" s="1">
         <v>6108966300</v>
@@ -3326,276 +3137,276 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="9" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="8" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>461</v>
+        <v>436</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
-        <v>392</v>
+        <v>367</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="20" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="20" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="4" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="15" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="8" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" s="21" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" s="8" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" s="20" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101" s="7" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102" s="4" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103" s="8" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" s="4" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" s="20" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" s="20" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" s="20" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" s="20" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109" s="20" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110" s="20" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111" s="4" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112" s="4" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="4" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="8" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" s="20" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="20" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="20" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="4" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>462</v>
+        <v>437</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" s="20" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="20" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" s="20" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>462</v>
+        <v>437</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>462</v>
+        <v>437</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" s="20" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="4" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>462</v>
+        <v>437</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" s="22" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" s="20" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>462</v>
+        <v>437</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" s="4" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>462</v>
+        <v>437</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" s="22" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" s="4" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="4" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>462</v>
+        <v>437</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" s="20" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" s="4" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -3604,12 +3415,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H124"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3623,130 +3434,130 @@
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
-        <v>199</v>
+        <v>174</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="F3" s="4"/>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="6" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>450</v>
+        <v>425</v>
       </c>
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>451</v>
+        <v>426</v>
       </c>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
-        <v>202</v>
+        <v>177</v>
       </c>
       <c r="D7" t="s">
-        <v>452</v>
+        <v>427</v>
       </c>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
-        <v>203</v>
+        <v>178</v>
       </c>
       <c r="D8" t="s">
-        <v>453</v>
+        <v>428</v>
       </c>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="D9" t="s">
-        <v>454</v>
+        <v>429</v>
       </c>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="D10"/>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="6" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>455</v>
+        <v>430</v>
       </c>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="4" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" s="4" t="s">
-        <v>389</v>
+        <v>364</v>
       </c>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
-        <v>390</v>
+        <v>365</v>
       </c>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B16" s="4" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="H17" s="4"/>
     </row>
@@ -3764,13 +3575,13 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B21" s="4" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" s="4" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="H22" s="4"/>
     </row>
@@ -3787,50 +3598,50 @@
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B26" s="4" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B27" s="4" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B28" s="4" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="H28" s="4"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B29" s="4" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="H29" s="4"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B30" s="4" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="H30" s="4"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B31" s="4" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B32" s="1" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B33" s="4" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B34" s="4" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.35">
@@ -3841,23 +3652,23 @@
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="H38" s="4"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B39" s="4" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B40" s="4" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B41" s="4" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.35">
@@ -3868,82 +3679,82 @@
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B44" s="4" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B45" s="4" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B46" s="4" t="s">
-        <v>396</v>
+        <v>371</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B47" s="4" t="s">
-        <v>395</v>
+        <v>370</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B48" s="4" t="s">
-        <v>394</v>
+        <v>369</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B49" s="4" t="s">
-        <v>393</v>
+        <v>368</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B50" s="4" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B51" s="1" t="s">
-        <v>208</v>
+        <v>183</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B52" s="1" t="s">
-        <v>397</v>
+        <v>372</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B53" s="1" t="s">
-        <v>398</v>
+        <v>373</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B54" s="1" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B55" s="4" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B56" s="4" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B57" s="1" t="s">
-        <v>271</v>
+        <v>246</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
-        <v>449</v>
+        <v>424</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B59" s="4" t="s">
-        <v>461</v>
+        <v>436</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.35">
@@ -3960,37 +3771,37 @@
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B64" s="4" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B65" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B66" s="4" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B67" s="4" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B68" s="4" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B69" s="4" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B70" s="4" t="s">
-        <v>448</v>
+        <v>423</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.35">
@@ -4001,32 +3812,32 @@
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B74" s="4" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B75" s="4" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B76" s="4" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B77" s="4" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B78" s="4" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B79" s="4" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.35">
@@ -4037,37 +3848,37 @@
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B82" s="12" t="s">
-        <v>382</v>
+        <v>357</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B83" s="12" t="s">
-        <v>458</v>
+        <v>433</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B84" s="12" t="s">
-        <v>383</v>
+        <v>358</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B85" s="6" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B86" s="6" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B87" s="4" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B88" s="4" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.35">
@@ -4075,78 +3886,78 @@
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B90" s="4" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>459</v>
+        <v>434</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B91" s="4" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B92" s="4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B93" s="4" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B94" s="4" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B95" s="4" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B96" s="4" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>460</v>
+        <v>435</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B97" s="4" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B98" s="4" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B99" s="4" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B100" s="4" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B101" s="1" t="s">
-        <v>272</v>
+        <v>247</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B102" s="9" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B103" s="4" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.35">
@@ -4154,72 +3965,72 @@
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B107" s="1" t="s">
-        <v>399</v>
+        <v>374</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B108" s="1" t="s">
-        <v>400</v>
+        <v>375</v>
       </c>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B109" s="1" t="s">
-        <v>401</v>
+        <v>376</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B110" s="1" t="s">
-        <v>402</v>
+        <v>377</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B111" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B112" s="1" t="s">
-        <v>403</v>
+        <v>378</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B113" s="1" t="s">
-        <v>404</v>
+        <v>379</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B115" s="1" t="s">
-        <v>405</v>
+        <v>380</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B116" s="1" t="s">
-        <v>362</v>
+        <v>337</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B117" s="1" t="s">
-        <v>406</v>
+        <v>381</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B118" s="1" t="s">
-        <v>407</v>
+        <v>382</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B122" s="4" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B123" s="1" t="s">
-        <v>456</v>
+        <v>431</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B124" s="1" t="s">
-        <v>457</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -4228,12 +4039,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="C2:F13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4247,400 +4058,412 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>212</v>
+        <v>187</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>213</v>
+        <v>188</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>214</v>
+        <v>189</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>215</v>
+        <v>190</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>214</v>
+        <v>189</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>216</v>
+        <v>191</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>217</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>215</v>
+        <v>190</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>221</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>216</v>
+        <v>191</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>217</v>
+        <v>192</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>241</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>228</v>
+        <v>203</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>242</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
-        <v>219</v>
+        <v>194</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>266</v>
+        <v>241</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>265</v>
+        <v>240</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>221</v>
+        <v>196</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>264</v>
+        <v>239</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>463</v>
+        <v>438</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>243</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>273</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>226</v>
+        <v>201</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>228</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>237</v>
+        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>239</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>241</v>
+        <v>216</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>242</v>
+        <v>217</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>245</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>246</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>249</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>250</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>252</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
-        <v>254</v>
+        <v>229</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
anagrams and few owthers
</commit_message>
<xml_diff>
--- a/interivew/practice/tracker.xlsx
+++ b/interivew/practice/tracker.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="511">
   <si>
     <t>LIS</t>
   </si>
@@ -1529,6 +1529,39 @@
   <si>
     <t>Write a program to find the first consecutive string of characters.
 ex: in 83d34cjk</t>
+  </si>
+  <si>
+    <t>How to design a tiny URL or URL shortener?(Long url to short url)</t>
+  </si>
+  <si>
+    <t>URLShortner</t>
+  </si>
+  <si>
+    <t>Reverse Matrix</t>
+  </si>
+  <si>
+    <t>Check If Two Rectangles Overlap</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>URL Shortner</t>
+  </si>
+  <si>
+    <t>Parking lot</t>
+  </si>
+  <si>
+    <t>Elevator</t>
+  </si>
+  <si>
+    <t>Phone book</t>
+  </si>
+  <si>
+    <t>Check if any anagram of string is palindrome.</t>
+  </si>
+  <si>
+    <t>Print all anagrams together.</t>
   </si>
 </sst>
 </file>
@@ -2059,7 +2092,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4363,8 +4396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4797,10 +4830,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K135"/>
+  <dimension ref="A1:L135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="H19" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4816,10 +4849,11 @@
     <col min="9" max="9" width="53.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="41.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="72.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="1"/>
+    <col min="12" max="12" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4853,8 +4887,11 @@
       <c r="K1" s="5" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" s="5" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>189</v>
       </c>
@@ -4888,8 +4925,11 @@
       <c r="K2" s="9" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L2" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>199</v>
       </c>
@@ -4923,8 +4963,11 @@
       <c r="K3" s="9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L3" s="1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>200</v>
       </c>
@@ -4958,8 +5001,11 @@
       <c r="K4" s="9" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L4" s="1" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>205</v>
       </c>
@@ -4993,8 +5039,11 @@
       <c r="K5" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L5" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>207</v>
       </c>
@@ -5028,8 +5077,11 @@
       <c r="K6" s="1" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L6" s="1" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>56</v>
       </c>
@@ -5061,7 +5113,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>237</v>
       </c>
@@ -5093,7 +5145,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>234</v>
       </c>
@@ -5125,7 +5177,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>238</v>
       </c>
@@ -5154,7 +5206,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>239</v>
       </c>
@@ -5179,8 +5231,11 @@
       <c r="J11" s="12" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K11" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>469</v>
       </c>
@@ -5206,7 +5261,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>1</v>
       </c>
@@ -5232,7 +5287,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>195</v>
       </c>
@@ -5257,8 +5312,11 @@
       <c r="J14" s="12" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K14" s="1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>190</v>
       </c>
@@ -5280,8 +5338,11 @@
       <c r="J15" s="12" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K15" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>240</v>
       </c>
@@ -5678,6 +5739,9 @@
       <c r="G31" s="12" t="s">
         <v>114</v>
       </c>
+      <c r="J31" s="1" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="22" t="s">
@@ -5701,8 +5765,11 @@
       <c r="G32" s="12" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J32" s="1" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="22" t="s">
         <v>213</v>
       </c>
@@ -5724,8 +5791,11 @@
       <c r="G33" s="12" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J33" s="1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>455</v>
       </c>
@@ -5748,7 +5818,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>244</v>
       </c>
@@ -5771,7 +5841,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>192</v>
       </c>
@@ -5794,7 +5864,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>484</v>
       </c>
@@ -5817,7 +5887,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>217</v>
       </c>
@@ -5837,7 +5907,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>218</v>
       </c>
@@ -5857,7 +5927,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>12</v>
       </c>
@@ -5874,7 +5944,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>216</v>
       </c>
@@ -5891,7 +5961,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>247</v>
       </c>
@@ -5908,7 +5978,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>242</v>
       </c>
@@ -5916,7 +5986,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="22" t="s">
         <v>243</v>
       </c>
@@ -5924,22 +5994,22 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F45" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F46" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F47" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F48" s="4" t="s">
         <v>52</v>
       </c>
@@ -6381,5 +6451,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
streams, trees and practice
</commit_message>
<xml_diff>
--- a/interivew/practice/tracker.xlsx
+++ b/interivew/practice/tracker.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="533">
   <si>
     <t>LIS</t>
   </si>
@@ -1599,6 +1599,36 @@
   <si>
     <t xml:space="preserve">Inorder Suc­ces­sor in Binary Search Tree with­out Using Par­ent link
 </t>
+  </si>
+  <si>
+    <t>CheckIfTreeIsSubsetOfAnotherTree</t>
+  </si>
+  <si>
+    <t>CheckIfTwoNodesAreSiblings</t>
+  </si>
+  <si>
+    <t>CheckIfTwoNodesAreCousins</t>
+  </si>
+  <si>
+    <t>PrintLeftViewOfTree</t>
+  </si>
+  <si>
+    <t>PrintRightViewOfTree</t>
+  </si>
+  <si>
+    <t>Given a binary tree, Print All the Nodes that don’t have Sib­lings.</t>
+  </si>
+  <si>
+    <t>SortedSingleLinkedListToBST</t>
+  </si>
+  <si>
+    <t>FindFirstNonRepeatingInStream</t>
+  </si>
+  <si>
+    <t>MedianInStreamOfIntegers</t>
+  </si>
+  <si>
+    <t>FindKthLargestInStream</t>
   </si>
 </sst>
 </file>
@@ -4880,8 +4910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="I23" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5383,7 +5413,7 @@
         <v>301</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>332</v>
+        <v>529</v>
       </c>
       <c r="F16" s="19" t="s">
         <v>22</v>
@@ -5409,7 +5439,7 @@
         <v>302</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>23</v>
@@ -5435,7 +5465,7 @@
         <v>393</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F18" s="20" t="s">
         <v>24</v>
@@ -5461,7 +5491,7 @@
         <v>303</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>147</v>
@@ -5489,8 +5519,8 @@
       <c r="C20" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>339</v>
+      <c r="D20" s="17" t="s">
+        <v>337</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>478</v>
@@ -5518,8 +5548,8 @@
       <c r="C21" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>338</v>
+      <c r="D21" s="2" t="s">
+        <v>339</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>474</v>
@@ -5545,7 +5575,7 @@
         <v>308</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>473</v>
@@ -5571,7 +5601,7 @@
         <v>307</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>475</v>
@@ -5596,8 +5626,8 @@
       <c r="C24" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>342</v>
+      <c r="D24" s="1" t="s">
+        <v>341</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>479</v>
@@ -5623,7 +5653,7 @@
         <v>309</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>477</v>
@@ -5648,8 +5678,8 @@
       <c r="C26" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>345</v>
+      <c r="D26" s="2" t="s">
+        <v>343</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>476</v>
@@ -5675,7 +5705,7 @@
         <v>311</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>482</v>
@@ -5700,8 +5730,8 @@
       <c r="C28" s="17" t="s">
         <v>395</v>
       </c>
-      <c r="D28" s="17" t="s">
-        <v>347</v>
+      <c r="D28" s="1" t="s">
+        <v>344</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>480</v>
@@ -5726,8 +5756,8 @@
       <c r="C29" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>346</v>
+      <c r="D29" s="17" t="s">
+        <v>347</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>481</v>
@@ -5752,8 +5782,8 @@
       <c r="C30" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="D30" s="17" t="s">
-        <v>384</v>
+      <c r="D30" s="1" t="s">
+        <v>346</v>
       </c>
       <c r="F30" s="20" t="s">
         <v>35</v>
@@ -5775,8 +5805,8 @@
       <c r="C31" s="17" t="s">
         <v>314</v>
       </c>
-      <c r="D31" s="18" t="s">
-        <v>389</v>
+      <c r="D31" s="17" t="s">
+        <v>384</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>36</v>
@@ -5799,7 +5829,7 @@
         <v>394</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>492</v>
@@ -5811,7 +5841,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="22" t="s">
         <v>213</v>
       </c>
@@ -5821,8 +5851,8 @@
       <c r="C33" s="17" t="s">
         <v>315</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>391</v>
+      <c r="D33" s="18" t="s">
+        <v>390</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>489</v>
@@ -5833,8 +5863,11 @@
       <c r="G33" s="12" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J33" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>455</v>
       </c>
@@ -5844,8 +5877,8 @@
       <c r="C34" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="D34" s="17" t="s">
-        <v>382</v>
+      <c r="D34" s="2" t="s">
+        <v>391</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>493</v>
@@ -5856,8 +5889,11 @@
       <c r="G34" s="4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J34" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>244</v>
       </c>
@@ -5867,8 +5903,8 @@
       <c r="C35" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>383</v>
+      <c r="D35" s="17" t="s">
+        <v>382</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>494</v>
@@ -5879,8 +5915,11 @@
       <c r="G35" s="12" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J35" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>192</v>
       </c>
@@ -5890,8 +5929,8 @@
       <c r="C36" s="23" t="s">
         <v>327</v>
       </c>
-      <c r="D36" s="18" t="s">
-        <v>385</v>
+      <c r="D36" s="1" t="s">
+        <v>383</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>495</v>
@@ -5903,7 +5942,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>484</v>
       </c>
@@ -5914,7 +5953,7 @@
         <v>319</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>496</v>
@@ -5926,7 +5965,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>217</v>
       </c>
@@ -5937,7 +5976,7 @@
         <v>318</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>43</v>
@@ -5946,7 +5985,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>218</v>
       </c>
@@ -5957,7 +5996,7 @@
         <v>396</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F39" s="14" t="s">
         <v>44</v>
@@ -5966,7 +6005,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>12</v>
       </c>
@@ -5976,6 +6015,9 @@
       <c r="C40" s="1" t="s">
         <v>320</v>
       </c>
+      <c r="D40" s="18" t="s">
+        <v>388</v>
+      </c>
       <c r="F40" s="4" t="s">
         <v>45</v>
       </c>
@@ -5983,7 +6025,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>216</v>
       </c>
@@ -6000,7 +6042,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>247</v>
       </c>
@@ -6017,7 +6059,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>242</v>
       </c>
@@ -6031,7 +6073,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="22" t="s">
         <v>243</v>
       </c>
@@ -6051,10 +6093,13 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B45" s="2" t="s">
         <v>515</v>
       </c>
+      <c r="C45" s="1" t="s">
+        <v>523</v>
+      </c>
       <c r="D45" s="1" t="s">
         <v>505</v>
       </c>
@@ -6065,10 +6110,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B46" s="33" t="s">
         <v>516</v>
       </c>
+      <c r="C46" s="1" t="s">
+        <v>524</v>
+      </c>
       <c r="D46" s="1" t="s">
         <v>506</v>
       </c>
@@ -6079,12 +6127,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B47" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="C47" s="32" t="s">
-        <v>522</v>
+      <c r="C47" s="1" t="s">
+        <v>525</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>507</v>
@@ -6093,12 +6141,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B48" s="33" t="s">
         <v>518</v>
       </c>
-      <c r="C48" s="33" t="s">
-        <v>521</v>
+      <c r="C48" t="s">
+        <v>527</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>508</v>
@@ -6111,6 +6159,9 @@
       <c r="B49" s="2" t="s">
         <v>519</v>
       </c>
+      <c r="C49" t="s">
+        <v>526</v>
+      </c>
       <c r="F49" s="26" t="s">
         <v>53</v>
       </c>
@@ -6140,17 +6191,26 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C55" s="32" t="s">
+        <v>522</v>
+      </c>
       <c r="F55" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C56" s="33" t="s">
+        <v>521</v>
+      </c>
       <c r="F56" s="20" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C57" s="1" t="s">
+        <v>528</v>
+      </c>
       <c r="F57" s="4" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
graphs, min heap and meeting rooms
</commit_message>
<xml_diff>
--- a/interivew/practice/tracker.xlsx
+++ b/interivew/practice/tracker.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1933" uniqueCount="740">
   <si>
     <t>LIS</t>
   </si>
@@ -2223,6 +2223,39 @@
   </si>
   <si>
     <t>RestoreIpAddress</t>
+  </si>
+  <si>
+    <t>MergeTwoArraysWithoutExtraSpace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FindKthSmallestInSortedMatrix </t>
+  </si>
+  <si>
+    <t>FindConflictingIntervalsWithPreviousIntervals</t>
+  </si>
+  <si>
+    <t>IntervalTree</t>
+  </si>
+  <si>
+    <t>MeetingRooms2(FindMinNumberOfConfRooms)</t>
+  </si>
+  <si>
+    <t>MeetingRooms(CheckPersonAttendAllMeetings)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>KruskalMST</t>
+  </si>
+  <si>
+    <t>PrimMST</t>
+  </si>
+  <si>
+    <t>TopologicalSort</t>
+  </si>
+  <si>
+    <t>Dijkstra</t>
   </si>
 </sst>
 </file>
@@ -7860,8 +7893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J13" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+    <sheetView tabSelected="1" topLeftCell="G5" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -7956,6 +7989,9 @@
         <v>549</v>
       </c>
       <c r="L2" s="4"/>
+      <c r="N2" s="4" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="4" t="s">
@@ -7992,6 +8028,9 @@
         <v>550</v>
       </c>
       <c r="L3" s="4"/>
+      <c r="N3" s="4" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
@@ -8028,6 +8067,9 @@
         <v>551</v>
       </c>
       <c r="L4" s="4"/>
+      <c r="N4" s="1" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="9" t="s">
@@ -8065,7 +8107,7 @@
       </c>
       <c r="L5" s="4"/>
       <c r="N5" s="4" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -8104,7 +8146,7 @@
       </c>
       <c r="L6" s="4"/>
       <c r="N6" s="4" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -8129,7 +8171,9 @@
       <c r="G7" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="H7" s="4"/>
+      <c r="H7" s="4" t="s">
+        <v>736</v>
+      </c>
       <c r="I7" s="4" t="s">
         <v>77</v>
       </c>
@@ -8140,8 +8184,8 @@
         <v>557</v>
       </c>
       <c r="L7" s="4"/>
-      <c r="N7" s="1" t="s">
-        <v>717</v>
+      <c r="N7" s="4" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -8166,7 +8210,9 @@
       <c r="G8" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="H8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>737</v>
+      </c>
       <c r="I8" s="4" t="s">
         <v>449</v>
       </c>
@@ -8178,7 +8224,7 @@
       </c>
       <c r="L8" s="4"/>
       <c r="N8" s="4" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -8203,7 +8249,9 @@
       <c r="G9" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="H9" s="4"/>
+      <c r="H9" s="4" t="s">
+        <v>738</v>
+      </c>
       <c r="I9" s="4" t="s">
         <v>445</v>
       </c>
@@ -8215,7 +8263,7 @@
       </c>
       <c r="L9" s="4"/>
       <c r="N9" s="4" t="s">
-        <v>476</v>
+        <v>735</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -8240,7 +8288,9 @@
       <c r="G10" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H10" s="4"/>
+      <c r="H10" s="4" t="s">
+        <v>739</v>
+      </c>
       <c r="I10" s="4" t="s">
         <v>567</v>
       </c>
@@ -8251,8 +8301,8 @@
         <v>579</v>
       </c>
       <c r="L10" s="4"/>
-      <c r="N10" s="4" t="s">
-        <v>482</v>
+      <c r="N10" s="1" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -8277,9 +8327,6 @@
       <c r="G11" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="H11" s="8" t="s">
-        <v>546</v>
-      </c>
       <c r="I11" s="41" t="s">
         <v>568</v>
       </c>
@@ -8291,7 +8338,7 @@
       </c>
       <c r="L11" s="4"/>
       <c r="N11" s="4" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -8316,9 +8363,6 @@
       <c r="G12" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>554</v>
-      </c>
       <c r="I12" s="41" t="s">
         <v>569</v>
       </c>
@@ -8330,7 +8374,7 @@
       </c>
       <c r="L12" s="4"/>
       <c r="N12" s="4" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -8355,9 +8399,6 @@
       <c r="G13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>540</v>
-      </c>
       <c r="I13" s="41" t="s">
         <v>570</v>
       </c>
@@ -8368,8 +8409,8 @@
         <v>658</v>
       </c>
       <c r="L13" s="4"/>
-      <c r="N13" s="1" t="s">
-        <v>653</v>
+      <c r="N13" s="4" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -8394,9 +8435,6 @@
       <c r="G14" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>561</v>
-      </c>
       <c r="I14" s="41" t="s">
         <v>571</v>
       </c>
@@ -8407,6 +8445,9 @@
         <v>578</v>
       </c>
       <c r="L14" s="4"/>
+      <c r="N14" s="1" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="4" t="s">
@@ -8428,9 +8469,6 @@
       <c r="G15" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="H15" s="4" t="s">
-        <v>562</v>
-      </c>
       <c r="I15" s="4" t="s">
         <v>502</v>
       </c>
@@ -8441,8 +8479,8 @@
         <v>659</v>
       </c>
       <c r="L15" s="4"/>
-      <c r="N15" s="4" t="s">
-        <v>478</v>
+      <c r="N15" s="1" t="s">
+        <v>705</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -8465,8 +8503,8 @@
       <c r="G16" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>566</v>
+      <c r="H16" s="8" t="s">
+        <v>546</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4" t="s">
@@ -8476,8 +8514,8 @@
         <v>663</v>
       </c>
       <c r="L16" s="4"/>
-      <c r="N16" s="4" t="s">
-        <v>474</v>
+      <c r="N16" s="1" t="s">
+        <v>706</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -8501,7 +8539,7 @@
         <v>40</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>563</v>
+        <v>554</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4" t="s">
@@ -8511,8 +8549,8 @@
         <v>707</v>
       </c>
       <c r="L17" s="4"/>
-      <c r="N17" s="4" t="s">
-        <v>473</v>
+      <c r="N17" s="1" t="s">
+        <v>708</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -8536,7 +8574,7 @@
         <v>36</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>576</v>
@@ -8549,7 +8587,7 @@
       </c>
       <c r="L18" s="4"/>
       <c r="N18" s="1" t="s">
-        <v>704</v>
+        <v>709</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -8572,7 +8610,7 @@
         <v>161</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="I19" s="41" t="s">
         <v>558</v>
@@ -8585,7 +8623,7 @@
       </c>
       <c r="L19" s="4"/>
       <c r="N19" s="1" t="s">
-        <v>705</v>
+        <v>710</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -8608,7 +8646,7 @@
         <v>75</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="I20" s="41" t="s">
         <v>559</v>
@@ -8621,7 +8659,7 @@
       </c>
       <c r="L20" s="4"/>
       <c r="N20" s="1" t="s">
-        <v>706</v>
+        <v>711</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -8643,17 +8681,21 @@
       <c r="G21" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="H21" s="4"/>
+      <c r="H21" s="4" t="s">
+        <v>566</v>
+      </c>
       <c r="I21" s="41" t="s">
         <v>560</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="K21" s="4"/>
+      <c r="K21" s="4" t="s">
+        <v>731</v>
+      </c>
       <c r="L21" s="4"/>
       <c r="N21" s="1" t="s">
-        <v>708</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -8675,17 +8717,21 @@
       <c r="G22" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="H22" s="4"/>
+      <c r="H22" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="I22" s="41" t="s">
         <v>428</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="K22" s="4"/>
+      <c r="K22" s="4" t="s">
+        <v>732</v>
+      </c>
       <c r="L22" s="4"/>
       <c r="N22" s="1" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -8707,8 +8753,12 @@
       <c r="G23" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
+      <c r="H23" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>724</v>
+      </c>
       <c r="J23" s="4" t="s">
         <v>401</v>
       </c>
@@ -8717,7 +8767,7 @@
       </c>
       <c r="L23" s="4"/>
       <c r="N23" s="1" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -8739,7 +8789,9 @@
       <c r="G24" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="H24" s="4"/>
+      <c r="H24" s="4" t="s">
+        <v>564</v>
+      </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4" t="s">
         <v>403</v>
@@ -8749,7 +8801,7 @@
       </c>
       <c r="L24" s="4"/>
       <c r="N24" s="1" t="s">
-        <v>711</v>
+        <v>716</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -8771,15 +8823,19 @@
       <c r="G25" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="H25" s="4"/>
+      <c r="H25" s="4" t="s">
+        <v>565</v>
+      </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="K25" s="4"/>
+      <c r="K25" s="4" t="s">
+        <v>734</v>
+      </c>
       <c r="L25" s="4"/>
       <c r="N25" s="1" t="s">
-        <v>3</v>
+        <v>722</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -8806,10 +8862,12 @@
       <c r="J26" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="K26" s="4"/>
+      <c r="K26" s="4" t="s">
+        <v>733</v>
+      </c>
       <c r="L26" s="4"/>
       <c r="N26" s="1" t="s">
-        <v>712</v>
+        <v>725</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -8839,7 +8897,7 @@
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="N27" s="1" t="s">
-        <v>713</v>
+        <v>726</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -8869,7 +8927,7 @@
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="N28" s="1" t="s">
-        <v>716</v>
+        <v>728</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -8898,9 +8956,6 @@
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
-      <c r="N29" s="1" t="s">
-        <v>722</v>
-      </c>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="4" t="s">
@@ -8929,9 +8984,6 @@
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
-      <c r="N30" s="1" t="s">
-        <v>725</v>
-      </c>
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="4" t="s">
@@ -8960,9 +9012,6 @@
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
-      <c r="N31" s="1" t="s">
-        <v>726</v>
-      </c>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="4" t="s">
@@ -8991,13 +9040,8 @@
       <c r="J32" s="4" t="s">
         <v>530</v>
       </c>
-      <c r="K32" s="4" t="s">
-        <v>662</v>
-      </c>
+      <c r="K32" s="4"/>
       <c r="L32" s="4"/>
-      <c r="N32" s="1" t="s">
-        <v>728</v>
-      </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="4" t="s">
@@ -9305,7 +9349,9 @@
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
+      <c r="J43" s="4" t="s">
+        <v>729</v>
+      </c>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
     </row>
@@ -9331,7 +9377,9 @@
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
+      <c r="J44" s="4" t="s">
+        <v>730</v>
+      </c>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
     </row>
@@ -9357,7 +9405,9 @@
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
+      <c r="J45" s="4" t="s">
+        <v>724</v>
+      </c>
       <c r="K45" s="4"/>
       <c r="L45" s="4"/>
     </row>
@@ -9381,7 +9431,9 @@
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
+      <c r="J46" s="4" t="s">
+        <v>662</v>
+      </c>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
     </row>

</xml_diff>